<commit_message>
[shanoir-ng-anonymization] keep "study date" and 'series date" not anonymized for OFSEP profile
</commit_message>
<xml_diff>
--- a/shanoir-ng-anonymization/src/main/resources/anonymization.xlsx
+++ b/shanoir-ng-anonymization/src/main/resources/anonymization.xlsx
@@ -3147,8 +3147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
-      <selection activeCell="G282" sqref="G282"/>
+    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
+      <selection activeCell="A264" sqref="A264:F264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8447,7 +8447,7 @@
         <v>4</v>
       </c>
       <c r="F264" s="9" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G264" s="9" t="s">
         <v>4</v>
@@ -8778,7 +8778,7 @@
         <v>3</v>
       </c>
       <c r="F281" s="9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G281" s="9" t="s">
         <v>7</v>
@@ -9317,7 +9317,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9427,8 +9427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="C22:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9938,10 +9938,10 @@
       <c r="B22" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="4" t="s">
         <v>637</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E22" s="28" t="s">

</xml_diff>

<commit_message>
refactor anonymization with singleton for loading xls file; added exclusion tag list in xls file new sheet; added fix to patient.birthdate during dicomdir deserialization and object mapping.
</commit_message>
<xml_diff>
--- a/shanoir-ng-anonymization/src/main/resources/anonymization.xlsx
+++ b/shanoir-ng-anonymization/src/main/resources/anonymization.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Feuil2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Feuil3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="ExcludePrivateTag" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Feuil2" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Feuil3" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2007" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2025" uniqueCount="839">
   <si>
     <t xml:space="preserve">Attribute Name</t>
   </si>
@@ -2300,6 +2301,57 @@
   </si>
   <si>
     <t xml:space="preserve">0x00384000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0019100A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0019100B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0019100C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0019100D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0019100E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0019100F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x00191027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x00191028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x00431039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x001910BB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x001910BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x001910BD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x00189087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x00189089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x00290011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x00291010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x00291020</t>
   </si>
   <si>
     <t xml:space="preserve">Legend</t>
@@ -2716,10 +2768,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2765,24 +2816,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor rgb="FFCCCCCC"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -2821,7 +2860,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2845,17 +2884,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2892,11 +2925,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2908,7 +2941,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2920,16 +2953,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2944,23 +2977,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2970,10 +2999,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2993,16 +3018,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Good" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Bad" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Accent2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3015,7 +3038,7 @@
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF9C0006"/>
-      <rgbColor rgb="FF006100"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
@@ -3040,12 +3063,12 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFC6EFCE"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFC7CE"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -3074,19 +3097,19 @@
   </sheetPr>
   <dimension ref="A1:G305"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B178" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G199" activeCellId="0" sqref="G199"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B187" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -3112,6 +3135,12 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -7078,7 +7107,7 @@
         <v>14</v>
       </c>
       <c r="G199" s="6" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9250,6 +9279,124 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:A18"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="14" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="14" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="14" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="14" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="14" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="17" t="s">
+        <v>774</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -9259,13 +9406,13 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="103.797570850202"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="109.473684210526"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
-        <v>758</v>
+      <c r="A1" s="18" t="s">
+        <v>775</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9273,7 +9420,7 @@
         <v>195</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>759</v>
+        <v>776</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9281,7 +9428,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>760</v>
+        <v>777</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9289,7 +9436,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>761</v>
+        <v>778</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9297,15 +9444,15 @@
         <v>22</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>762</v>
+        <v>779</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>763</v>
+        <v>780</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>764</v>
+        <v>781</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9313,7 +9460,7 @@
         <v>81</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>765</v>
+        <v>782</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9321,7 +9468,7 @@
         <v>94</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>766</v>
+        <v>783</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9329,7 +9476,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>767</v>
+        <v>784</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9337,7 +9484,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>768</v>
+        <v>785</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9345,7 +9492,7 @@
         <v>143</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>769</v>
+        <v>786</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9353,7 +9500,7 @@
         <v>517</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>770</v>
+        <v>787</v>
       </c>
     </row>
   </sheetData>
@@ -9367,7 +9514,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -9380,17 +9527,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.6315789473684"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.2834008097166"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.8137651821862"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.7773279352227"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.5991902834008"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="59.3441295546559"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="49.0607287449393"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.7773279352227"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.1012145748988"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.8866396761134"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="62.4493927125506"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="51.5222672064777"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -9408,22 +9555,22 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>771</v>
+        <v>788</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>772</v>
+        <v>789</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>773</v>
+        <v>790</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>774</v>
+        <v>791</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>775</v>
+        <v>792</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>776</v>
+        <v>793</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9439,14 +9586,14 @@
       <c r="D5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>777</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>778</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>779</v>
+      <c r="E5" s="6" t="s">
+        <v>794</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>795</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>796</v>
       </c>
       <c r="H5" s="6" t="n">
         <v>3</v>
@@ -9455,7 +9602,7 @@
         <v>21</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>780</v>
+        <v>797</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9471,14 +9618,14 @@
       <c r="D6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>777</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>778</v>
+      <c r="E6" s="6" t="s">
+        <v>794</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>795</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>779</v>
+        <v>796</v>
       </c>
       <c r="H6" s="12" t="n">
         <v>3</v>
@@ -9487,7 +9634,7 @@
         <v>26</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>780</v>
+        <v>797</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9504,7 +9651,7 @@
         <v>26</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>781</v>
+        <v>798</v>
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
@@ -9513,7 +9660,7 @@
         <v>26</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>782</v>
+        <v>799</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9530,13 +9677,13 @@
         <v>21</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>777</v>
+        <v>794</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>778</v>
+        <v>795</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>779</v>
+        <v>796</v>
       </c>
       <c r="H8" s="12" t="n">
         <v>3</v>
@@ -9545,7 +9692,7 @@
         <v>21</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>780</v>
+        <v>797</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9562,25 +9709,25 @@
         <v>94</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>777</v>
+        <v>794</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>778</v>
+        <v>795</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>779</v>
+        <v>796</v>
       </c>
       <c r="H9" s="23" t="s">
-        <v>783</v>
+        <v>800</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>784</v>
+        <v>801</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>94</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>785</v>
+        <v>802</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9597,25 +9744,25 @@
         <v>94</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>777</v>
+        <v>794</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>778</v>
+        <v>795</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>779</v>
+        <v>796</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>783</v>
+        <v>800</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>786</v>
+        <v>803</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>94</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>785</v>
+        <v>802</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9632,13 +9779,13 @@
         <v>94</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>787</v>
+        <v>804</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>788</v>
+        <v>805</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>789</v>
+        <v>806</v>
       </c>
       <c r="H11" s="24" t="n">
         <v>2</v>
@@ -9647,7 +9794,7 @@
         <v>94</v>
       </c>
       <c r="K11" s="24" t="s">
-        <v>785</v>
+        <v>802</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9664,13 +9811,13 @@
         <v>143</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>790</v>
+        <v>807</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>791</v>
+        <v>808</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>779</v>
+        <v>796</v>
       </c>
       <c r="H12" s="12" t="n">
         <v>3</v>
@@ -9679,7 +9826,7 @@
         <v>143</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>780</v>
+        <v>797</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9702,7 +9849,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>792</v>
+        <v>809</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>227</v>
@@ -9714,7 +9861,7 @@
         <v>143</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>781</v>
+        <v>798</v>
       </c>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
@@ -9723,7 +9870,7 @@
         <v>143</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>782</v>
+        <v>799</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9740,13 +9887,13 @@
         <v>143</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>790</v>
+        <v>807</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>791</v>
+        <v>808</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>779</v>
+        <v>796</v>
       </c>
       <c r="H16" s="12" t="n">
         <v>3</v>
@@ -9755,7 +9902,7 @@
         <v>143</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>780</v>
+        <v>797</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9763,13 +9910,13 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="20" t="s">
-        <v>793</v>
+        <v>810</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>794</v>
+        <v>811</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>779</v>
+        <v>796</v>
       </c>
       <c r="H17" s="12" t="n">
         <v>3</v>
@@ -9791,13 +9938,13 @@
         <v>26</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>795</v>
+        <v>812</v>
       </c>
       <c r="F18" s="20" t="s">
+        <v>813</v>
+      </c>
+      <c r="G18" s="20" t="s">
         <v>796</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>779</v>
       </c>
       <c r="H18" s="12" t="n">
         <v>3</v>
@@ -9806,7 +9953,7 @@
         <v>26</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>780</v>
+        <v>797</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9814,13 +9961,13 @@
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="20" t="s">
-        <v>793</v>
+        <v>810</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>794</v>
+        <v>811</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>779</v>
+        <v>796</v>
       </c>
       <c r="H19" s="12" t="n">
         <v>3</v>
@@ -9842,13 +9989,13 @@
         <v>143</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>795</v>
+        <v>812</v>
       </c>
       <c r="F20" s="20" t="s">
+        <v>813</v>
+      </c>
+      <c r="G20" s="20" t="s">
         <v>796</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>779</v>
       </c>
       <c r="H20" s="12" t="n">
         <v>3</v>
@@ -9857,7 +10004,7 @@
         <v>143</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>780</v>
+        <v>797</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9865,13 +10012,13 @@
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="20" t="s">
-        <v>793</v>
+        <v>810</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>794</v>
+        <v>811</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>779</v>
+        <v>796</v>
       </c>
       <c r="H21" s="12" t="n">
         <v>3</v>
@@ -9880,7 +10027,7 @@
       <c r="K21" s="12"/>
     </row>
     <row r="22" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="21" t="s">
         <v>370</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -9893,25 +10040,25 @@
         <v>21</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>797</v>
+        <v>814</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>798</v>
+        <v>815</v>
       </c>
       <c r="G22" s="23" t="s">
         <v>81</v>
       </c>
       <c r="H22" s="23" t="s">
-        <v>783</v>
+        <v>800</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>799</v>
+        <v>816</v>
       </c>
       <c r="J22" s="12" t="s">
         <v>21</v>
       </c>
       <c r="K22" s="15" t="s">
-        <v>800</v>
+        <v>817</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9928,13 +10075,13 @@
         <v>26</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>795</v>
+        <v>812</v>
       </c>
       <c r="F23" s="20" t="s">
+        <v>813</v>
+      </c>
+      <c r="G23" s="20" t="s">
         <v>796</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>779</v>
       </c>
       <c r="H23" s="12" t="n">
         <v>3</v>
@@ -9943,7 +10090,7 @@
         <v>26</v>
       </c>
       <c r="K23" s="12" t="s">
-        <v>780</v>
+        <v>797</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9960,13 +10107,13 @@
         <v>517</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>777</v>
+        <v>794</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>778</v>
+        <v>795</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>779</v>
+        <v>796</v>
       </c>
       <c r="H24" s="12" t="n">
         <v>3</v>
@@ -9975,7 +10122,7 @@
         <v>517</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>780</v>
+        <v>797</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9992,13 +10139,13 @@
         <v>143</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>795</v>
+        <v>812</v>
       </c>
       <c r="F25" s="20" t="s">
+        <v>813</v>
+      </c>
+      <c r="G25" s="20" t="s">
         <v>796</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>779</v>
       </c>
       <c r="H25" s="12" t="n">
         <v>3</v>
@@ -10007,7 +10154,7 @@
         <v>143</v>
       </c>
       <c r="K25" s="12" t="s">
-        <v>780</v>
+        <v>797</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10024,13 +10171,13 @@
         <v>21</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>801</v>
+        <v>818</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>802</v>
+        <v>819</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>779</v>
+        <v>796</v>
       </c>
       <c r="H26" s="12" t="n">
         <v>3</v>
@@ -10039,7 +10186,7 @@
         <v>21</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>780</v>
+        <v>797</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10056,7 +10203,7 @@
         <v>21</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>781</v>
+        <v>798</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
@@ -10065,7 +10212,7 @@
         <v>21</v>
       </c>
       <c r="K27" s="12" t="s">
-        <v>782</v>
+        <v>799</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10082,7 +10229,7 @@
         <v>21</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>781</v>
+        <v>798</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
@@ -10091,7 +10238,7 @@
         <v>21</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>782</v>
+        <v>799</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10108,13 +10255,13 @@
         <v>26</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>795</v>
+        <v>812</v>
       </c>
       <c r="F29" s="20" t="s">
+        <v>813</v>
+      </c>
+      <c r="G29" s="20" t="s">
         <v>796</v>
-      </c>
-      <c r="G29" s="20" t="s">
-        <v>779</v>
       </c>
       <c r="H29" s="12" t="n">
         <v>3</v>
@@ -10123,7 +10270,7 @@
         <v>26</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>780</v>
+        <v>797</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10140,13 +10287,13 @@
         <v>26</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>795</v>
+        <v>812</v>
       </c>
       <c r="F30" s="20" t="s">
+        <v>813</v>
+      </c>
+      <c r="G30" s="20" t="s">
         <v>796</v>
-      </c>
-      <c r="G30" s="20" t="s">
-        <v>779</v>
       </c>
       <c r="H30" s="12" t="n">
         <v>3</v>
@@ -10155,7 +10302,7 @@
         <v>26</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>780</v>
+        <v>797</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10172,13 +10319,13 @@
         <v>517</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>777</v>
+        <v>794</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>778</v>
+        <v>795</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>779</v>
+        <v>796</v>
       </c>
       <c r="H31" s="12" t="n">
         <v>3</v>
@@ -10187,7 +10334,7 @@
         <v>517</v>
       </c>
       <c r="K31" s="12" t="s">
-        <v>780</v>
+        <v>797</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10204,13 +10351,13 @@
         <v>143</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>790</v>
+        <v>807</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>791</v>
+        <v>808</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>779</v>
+        <v>796</v>
       </c>
       <c r="H32" s="12" t="n">
         <v>3</v>
@@ -10219,129 +10366,129 @@
         <v>143</v>
       </c>
       <c r="K32" s="12" t="s">
-        <v>780</v>
+        <v>797</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="20" t="s">
-        <v>793</v>
+        <v>810</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>794</v>
+        <v>811</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>779</v>
+        <v>796</v>
       </c>
       <c r="H33" s="12" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="26" t="s">
-        <v>803</v>
+      <c r="A38" s="25" t="s">
+        <v>820</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="27" t="s">
-        <v>804</v>
+      <c r="A39" s="26" t="s">
+        <v>821</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="7" t="s">
-        <v>805</v>
+        <v>822</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7" t="s">
-        <v>806</v>
+        <v>823</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="26" t="s">
-        <v>773</v>
+      <c r="A43" s="25" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>807</v>
+        <v>824</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>808</v>
+        <v>825</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>809</v>
+        <v>826</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="26" t="s">
-        <v>810</v>
+      <c r="A49" s="25" t="s">
+        <v>827</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="28" t="s">
-        <v>811</v>
+      <c r="A51" s="27" t="s">
+        <v>828</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="29" t="s">
-        <v>812</v>
+      <c r="A52" s="26" t="s">
+        <v>829</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="30" t="s">
-        <v>813</v>
+      <c r="A53" s="28" t="s">
+        <v>830</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="29" t="s">
-        <v>814</v>
+      <c r="A54" s="26" t="s">
+        <v>831</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="29" t="s">
-        <v>815</v>
+      <c r="A55" s="26" t="s">
+        <v>832</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="31"/>
+      <c r="A56" s="29"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="32" t="s">
-        <v>816</v>
+      <c r="A57" s="30" t="s">
+        <v>833</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="29" t="s">
-        <v>817</v>
+      <c r="A58" s="26" t="s">
+        <v>834</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="33" t="s">
-        <v>818</v>
+      <c r="A59" s="31" t="s">
+        <v>835</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>813</v>
+        <v>830</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>819</v>
+        <v>836</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="17" t="s">
-        <v>820</v>
+      <c r="A63" s="18" t="s">
+        <v>837</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="33" t="s">
-        <v>821</v>
+      <c r="A64" s="31" t="s">
+        <v>838</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
* Import from PACS finished: introduced DicomStoreSCPServer and download of files from PACS * Big refactoring and class diagram added: /docs/Import/Class_Diagram_MS_Import.png, better separated components now     * ImportManagerService introduced (see #56)     * Each import for each user is in a userId specific folder now (no way to change this: higher security) * GitHub Issue #70 solved: subject name now in dicom files and therefore in PACS as well * GitHub Issue #56 solved: import is now asynchronous * SeriesDate set to keep in anonymization.xlsx, StudyDate is kept as well (same date) * Empty DicomEquipment bug fixed after refactoring
</commit_message>
<xml_diff>
--- a/shanoir-ng-anonymization/src/main/resources/anonymization.xlsx
+++ b/shanoir-ng-anonymization/src/main/resources/anonymization.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="991"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21940" tabRatio="991"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -3321,8 +3321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="B252" workbookViewId="0">
+      <selection activeCell="F265" sqref="F265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7939,7 +7939,7 @@
         <v>12</v>
       </c>
       <c r="F264" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="265" spans="1:6">

</xml_diff>

<commit_message>
* Keycloak connection of ShUp     * Missing protocolMappers attributes added into Keycloak realm config for client „shanoir-uploader"     * Fixes: NullPointerException for userId in the backend * anonymization module     * Tag.ProtocolName added as „KEEP“ to avoid missing attribute conflicts coming from ShUp after the anonymization * Import MS     * API + Controller extended with         * createTempDir method * ShUp     * ImportFinishRunnableNG introduced     * profile.properties extended for createTempDir
</commit_message>
<xml_diff>
--- a/shanoir-ng-anonymization/src/main/resources/anonymization.xlsx
+++ b/shanoir-ng-anonymization/src/main/resources/anonymization.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22160" tabRatio="991"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15880" tabRatio="991"/>
   </bookViews>
   <sheets>
     <sheet name="Profiles" sheetId="1" r:id="rId1"/>
@@ -2935,9 +2935,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="34">
+  <cellStyleXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3056,7 +3058,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="34">
+  <cellStyles count="36">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -3074,6 +3076,7 @@
     <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -3090,6 +3093,7 @@
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3489,8 +3493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A182" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C186" sqref="C186"/>
+    <sheetView tabSelected="1" topLeftCell="A192" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F203" sqref="F203:G203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7546,11 +7550,11 @@
       <c r="E203" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F203" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G203" s="5" t="s">
-        <v>11</v>
+      <c r="F203" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="G203" s="26" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="204" spans="1:7">
@@ -9743,7 +9747,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
bolus start & stop time K for Neur*** profile
</commit_message>
<xml_diff>
--- a/shanoir-ng-anonymization/src/main/resources/anonymization.xlsx
+++ b/shanoir-ng-anonymization/src/main/resources/anonymization.xlsx
@@ -6470,11 +6470,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A278" activeCellId="0" sqref="A278"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C68" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I81" activeCellId="0" sqref="I81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.57"/>
@@ -8396,13 +8396,13 @@
         <v>15</v>
       </c>
       <c r="E81" s="10" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F81" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G81" s="10" t="s">
-        <v>15</v>
+      <c r="G81" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="AMI81" s="0"/>
       <c r="AMJ81" s="0"/>
@@ -8421,13 +8421,13 @@
         <v>15</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F82" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G82" s="10" t="s">
-        <v>15</v>
+      <c r="G82" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="AMI82" s="0"/>
       <c r="AMJ82" s="0"/>
@@ -21908,7 +21908,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="171.51"/>
   </cols>
@@ -22028,7 +22028,7 @@
       <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.15"/>

</xml_diff>